<commit_message>
Add: tables of products information in pdf files
</commit_message>
<xml_diff>
--- a/invoices/10003-2023.1.18.xlsx
+++ b/invoices/10003-2023.1.18.xlsx
@@ -61,7 +61,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -285,13 +285,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,7 +605,7 @@
     <col min="2" max="2" style="24" width="20.14785714285714" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="23" width="16.290714285714284" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="25" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="25" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="24" width="16.290714285714284" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="24" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -622,12 +622,12 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="5">
         <v>1883191</v>
       </c>
@@ -645,7 +645,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A3" s="5">
         <v>1091919</v>
       </c>
@@ -663,7 +663,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A4" s="12">
         <v>7100190</v>
       </c>
@@ -681,7 +681,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A5" s="16"/>
       <c r="B5" s="6"/>
       <c r="C5" s="16"/>
@@ -689,7 +689,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A6" s="16"/>
       <c r="B6" s="6"/>
       <c r="C6" s="16"/>
@@ -697,7 +697,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A7" s="16"/>
       <c r="B7" s="6"/>
       <c r="C7" s="16"/>
@@ -705,7 +705,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A8" s="16"/>
       <c r="B8" s="6"/>
       <c r="C8" s="16"/>
@@ -713,7 +713,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>

</xml_diff>